<commit_message>
Do not repeat code
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="openAccount" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -370,11 +370,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -413,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>

</xml_diff>